<commit_message>
add modal for table, fake obj data
</commit_message>
<xml_diff>
--- a/public/excel/templateFile.xlsx
+++ b/public/excel/templateFile.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,61 +8,280 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hod Cohen\Desktop\group4-cli\public\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EEE6604D-3EDC-43D2-8517-FA81C1EF8E2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C1D55A70-778A-4FAE-B291-65CFCA30969B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8DEC43AD-61E6-4433-8551-0447A97351B1}"/>
+    <workbookView xWindow="1740" yWindow="5184" windowWidth="17280" windowHeight="8916"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Name:</t>
-  </si>
-  <si>
-    <t>Email:</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+  <si>
+    <t>full_name</t>
+  </si>
+  <si>
+    <t>english_name</t>
+  </si>
+  <si>
+    <t>picture</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>current_company</t>
+  </si>
+  <si>
+    <t>years_of_experience</t>
+  </si>
+  <si>
+    <t>linkedin_url</t>
+  </si>
+  <si>
+    <t>facebook_url</t>
+  </si>
+  <si>
+    <t>community_value</t>
+  </si>
+  <si>
+    <t>additional_info</t>
+  </si>
+  <si>
+    <t>skills</t>
+  </si>
+  <si>
+    <t>wants_updates</t>
+  </si>
+  <si>
+    <t>admin_notes</t>
+  </si>
+  <si>
+    <t>jobs_histroy</t>
+  </si>
+  <si>
+    <t>groups</t>
+  </si>
+  <si>
+    <t>events</t>
+  </si>
+  <si>
+    <t>ישראל ישראלי</t>
+  </si>
+  <si>
+    <t>Isreal</t>
+  </si>
+  <si>
+    <t>https://animalfactguide.com/wp-content/uploads/2025/03/panda-closeup.jpg</t>
+  </si>
+  <si>
+    <t>052-7975787</t>
+  </si>
+  <si>
+    <t>you@gmail</t>
+  </si>
+  <si>
+    <t>aco</t>
+  </si>
+  <si>
+    <t>devops</t>
+  </si>
+  <si>
+    <t>fox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.linkedin.com/in/nerya-reznickovich
+</t>
+  </si>
+  <si>
+    <t>facebook123</t>
+  </si>
+  <si>
+    <t>mentor</t>
+  </si>
+  <si>
+    <t>teacher of cs</t>
+  </si>
+  <si>
+    <t>docker, python</t>
+  </si>
+  <si>
+    <t>TRUE/FALSE</t>
+  </si>
+  <si>
+    <t>yes/no</t>
+  </si>
+  <si>
+    <t>fox, apple, youtube</t>
+  </si>
+  <si>
+    <t>menachem, yosi</t>
+  </si>
+  <si>
+    <t>meetup, bootcamp, party</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="16">
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Liberation Sans"/>
+    </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF0000EE"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF3D3D3D"/>
+      <name val="Ubuntu Sans"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Liberation Serif"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF808080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FFCC0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -70,15 +289,71 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="20">
+    <cellStyle name="Accent" xfId="7"/>
+    <cellStyle name="Accent 1" xfId="8"/>
+    <cellStyle name="Accent 2" xfId="9"/>
+    <cellStyle name="Accent 3" xfId="10"/>
+    <cellStyle name="Bad" xfId="4" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Default" xfId="11"/>
+    <cellStyle name="Error" xfId="12"/>
+    <cellStyle name="Footnote" xfId="13"/>
+    <cellStyle name="Good" xfId="3" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading" xfId="14"/>
+    <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="2" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="15"/>
+    <cellStyle name="Neutral" xfId="5" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="6" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Result" xfId="16"/>
+    <cellStyle name="Status" xfId="17"/>
+    <cellStyle name="Text" xfId="18"/>
+    <cellStyle name="Warning" xfId="19"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -389,24 +664,183 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59C8E530-64EE-4C57-B252-E1EE850F5455}">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="58.44140625" customWidth="1"/>
+    <col min="4" max="7" width="11.88671875" customWidth="1"/>
+    <col min="8" max="8" width="18.109375" customWidth="1"/>
+    <col min="9" max="9" width="17.44140625" customWidth="1"/>
+    <col min="10" max="10" width="34" customWidth="1"/>
+    <col min="11" max="11" width="12.5546875" customWidth="1"/>
+    <col min="12" max="12" width="15.6640625" customWidth="1"/>
+    <col min="13" max="13" width="16.33203125" customWidth="1"/>
+    <col min="14" max="14" width="13.5546875" customWidth="1"/>
+    <col min="15" max="15" width="14.109375" customWidth="1"/>
+    <col min="16" max="16" width="11.88671875" customWidth="1"/>
+    <col min="17" max="17" width="17.109375" customWidth="1"/>
+    <col min="18" max="18" width="15.5546875" customWidth="1"/>
+    <col min="19" max="19" width="23.44140625" customWidth="1"/>
+    <col min="20" max="20" width="8.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:19">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="1">
+        <v>7</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0" right="0" top="0.39370000000000005" bottom="0.39370000000000005" header="0" footer="0"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2"/>
+  <cols>
+    <col min="1" max="1" width="11.88671875" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0" right="0" top="0.39370000000000005" bottom="0.39370000000000005" header="0" footer="0"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>